<commit_message>
Some fixes in source generation logic
</commit_message>
<xml_diff>
--- a/data/runbunch/data.xlsx
+++ b/data/runbunch/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,6 @@
     <sheet name="Area-Demand" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -568,6 +567,15 @@
   </cellStyles>
   <dxfs count="13">
     <dxf>
+      <border>
+        <top style="thin">
+          <color theme="0" tint="-0.499984740745262"/>
+        </top>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <color theme="6" tint="0.59996337778862885"/>
       </font>
@@ -586,15 +594,6 @@
         <b/>
         <i val="0"/>
       </font>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="0" tint="-0.499984740745262"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
     </dxf>
     <dxf>
       <font>
@@ -1349,11 +1348,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2:I4"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1596,7 +1595,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A5" sqref="A5:G5"/>
+      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1862,7 +1861,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A18" sqref="A18:D20"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2282,15 +2281,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:D11">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2355,7 +2354,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A2" sqref="A2:D6"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2465,7 +2464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2580,7 +2579,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Correct value in data.xls. Add email notification to runbunch
</commit_message>
<xml_diff>
--- a/data/runbunch/data.xlsx
+++ b/data/runbunch/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -325,7 +325,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -507,7 +507,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -557,9 +557,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -988,7 +985,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1345,14 +1342,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1480,9 +1477,8 @@
       <c r="E4" s="3">
         <v>8</v>
       </c>
-      <c r="F4" s="37" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+      <c r="F4" s="36">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="G4" s="8">
         <v>2.0000000000000001E-4</v>
@@ -1588,7 +1584,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1643,7 +1639,7 @@
       <c r="C2" s="3">
         <v>100</v>
       </c>
-      <c r="D2" s="38">
+      <c r="D2" s="37">
         <v>50</v>
       </c>
       <c r="E2" s="25">
@@ -1669,7 +1665,7 @@
       <c r="C3" s="3">
         <v>250</v>
       </c>
-      <c r="D3" s="38">
+      <c r="D3" s="37">
         <v>100</v>
       </c>
       <c r="E3" s="25">
@@ -1695,7 +1691,7 @@
       <c r="C4" s="3">
         <v>180</v>
       </c>
-      <c r="D4" s="38">
+      <c r="D4" s="37">
         <v>75</v>
       </c>
       <c r="E4" s="25">
@@ -1721,7 +1717,7 @@
       <c r="C5" s="3">
         <v>250</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <v>100</v>
       </c>
       <c r="E5" s="25">
@@ -1744,7 +1740,7 @@
       <c r="C6" s="3">
         <v>60</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>60</v>
       </c>
       <c r="E6" s="25">
@@ -1770,7 +1766,7 @@
       <c r="C7" s="3">
         <v>150</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="37">
         <v>50</v>
       </c>
       <c r="E7" s="25">
@@ -1796,7 +1792,7 @@
       <c r="C8" s="3">
         <v>40</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="37">
         <v>40</v>
       </c>
       <c r="E8" s="25">
@@ -1841,12 +1837,12 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="E1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="F1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="G1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific fixed costs (€/kW)" prompt="Size-dependent part for maintaining a plant." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Fixed investment costs (€)" prompt="Up-front investment for building a plant, independent of size._x000a_Has value zero mainly for small-scale technologies." sqref="B1" xr:uid="{00000000-0002-0000-0200-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific investment costs (€/kW)" prompt="Size-dependent part for building a plant." sqref="C1" xr:uid="{00000000-0002-0000-0200-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Variable costs (€/kWh)" prompt="Operational costs to produce one unit of output, excluding fuel costs. Has value zero e.g. for PV or wind turbines (or if no sources are available)." sqref="E1" xr:uid="{00000000-0002-0000-0200-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Minimum capacity (kW)" prompt="Smallest size a plant is typically available in. Has value zero for domestic technologies." sqref="F1" xr:uid="{00000000-0002-0000-0200-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Maximum capacity (kW)" prompt="Biggest capacity a plant typically is available in." sqref="G1" xr:uid="{00000000-0002-0000-0200-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Specific fixed costs (€/kW)" prompt="Size-dependent part for maintaining a plant." sqref="D1" xr:uid="{00000000-0002-0000-0200-000005000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1854,7 +1850,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2294,7 +2290,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Input/output ratio (kWh/kWh)" prompt="Relative power flows in and out of processes. Sum of In and sum of Out should be equal to 1._x000a_For CO2, unit is kg/kWh." sqref="D1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2347,7 +2343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -2461,7 +2457,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">

</xml_diff>

<commit_message>
Delete Waste and Co. from runbunch data
</commit_message>
<xml_diff>
--- a/data/runbunch/data.xlsx
+++ b/data/runbunch/data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="66">
   <si>
     <t>Commodity</t>
   </si>
@@ -164,15 +164,6 @@
   </si>
   <si>
     <t>residential</t>
-  </si>
-  <si>
-    <t>commercial</t>
-  </si>
-  <si>
-    <t>industrial</t>
-  </si>
-  <si>
-    <t>other</t>
   </si>
   <si>
     <t>Area</t>
@@ -265,18 +256,12 @@
     <t>Gas heating domestic</t>
   </si>
   <si>
-    <t>Waste incineration plant</t>
-  </si>
-  <si>
     <t>In Richter: GT (gas turbine), DT (steam turbine), so maybe split into two processes as well</t>
   </si>
   <si>
     <t>not mendioned</t>
   </si>
   <si>
-    <t>Waste</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -287,9 +272,6 @@
   </si>
   <si>
     <t>in Richter: BK</t>
-  </si>
-  <si>
-    <t>in Richter: MV</t>
   </si>
   <si>
     <t>cost-fix</t>
@@ -1025,7 +1007,7 @@
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="14"/>
       <c r="C4" s="18" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D4" s="16"/>
       <c r="E4" s="16"/>
@@ -1060,7 +1042,7 @@
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="19"/>
       <c r="C7" s="28" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -1159,7 +1141,7 @@
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="19"/>
       <c r="C14" s="28" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
@@ -1176,7 +1158,7 @@
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10"/>
@@ -1206,7 +1188,7 @@
       </c>
       <c r="D17" s="10"/>
       <c r="E17" s="10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
@@ -1343,13 +1325,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1377,7 +1359,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>8</v>
@@ -1392,7 +1374,7 @@
         <v>17</v>
       </c>
       <c r="J1" s="35" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1530,45 +1512,11 @@
         <v>#N/A</v>
       </c>
       <c r="J5" s="29" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="I6" s="29" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="29" t="e">
-        <f>NA()</f>
-        <v>#N/A</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:XFD1 A5:XFD1048576 A2:B4 J2:XFD4">
+  <conditionalFormatting sqref="A1:XFD1 A2:B4 J2:XFD4 A5:XFD1048576">
     <cfRule type="containsErrors" dxfId="12" priority="2">
       <formula>ISERROR(A1)</formula>
     </cfRule>
@@ -1585,13 +1533,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I5" sqref="I5"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1614,7 +1562,7 @@
         <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>8</v>
@@ -1626,12 +1574,12 @@
         <v>17</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="32">
         <v>20000</v>
@@ -1646,18 +1594,18 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F2" s="32">
-        <v>10000</v>
+        <v>2000</v>
       </c>
       <c r="G2" s="32">
         <v>600000</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B3" s="32">
         <v>0</v>
@@ -1678,12 +1626,12 @@
         <v>50000</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B4" s="32">
         <v>25000</v>
@@ -1704,12 +1652,12 @@
         <v>150000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B5" s="32">
         <v>0</v>
@@ -1718,7 +1666,7 @@
         <v>250</v>
       </c>
       <c r="D5" s="37">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E5" s="25">
         <v>0.1</v>
@@ -1732,7 +1680,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B6" s="32">
         <v>30000</v>
@@ -1753,12 +1701,12 @@
         <v>500000</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="32">
         <v>25000</v>
@@ -1779,12 +1727,12 @@
         <v>350000</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="32">
         <v>0</v>
@@ -1806,33 +1754,7 @@
         <v>50000</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="32">
-        <v>9000</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0</v>
-      </c>
-      <c r="F9" s="32">
-        <v>0</v>
-      </c>
-      <c r="G9" s="32">
-        <v>0</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1851,13 +1773,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1884,7 +1806,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -1898,7 +1820,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1912,7 +1834,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1926,7 +1848,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -1940,7 +1862,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -1954,7 +1876,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -1968,7 +1890,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>2</v>
@@ -1982,7 +1904,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1996,7 +1918,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>2</v>
@@ -2010,7 +1932,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -2024,7 +1946,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
@@ -2038,7 +1960,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>2</v>
@@ -2052,7 +1974,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>6</v>
@@ -2066,7 +1988,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -2080,7 +2002,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>3</v>
@@ -2094,7 +2016,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>6</v>
@@ -2108,7 +2030,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>1</v>
@@ -2122,7 +2044,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>3</v>
@@ -2136,7 +2058,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -2146,62 +2068,6 @@
       </c>
       <c r="D20" s="6">
         <v>0.03</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D22" s="6">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="6">
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D24" s="6">
-        <v>0.55000000000000004</v>
       </c>
     </row>
   </sheetData>
@@ -2219,7 +2085,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD5 A8:XFD9 B7:C7 E7:XFD7 B6:XFD6 A12:XFD1048576 E10:XFD11">
+  <conditionalFormatting sqref="A1:XFD5 A8:XFD9 B7:C7 E7:XFD7 B6:XFD6 E10:XFD11 A12:XFD1048576">
     <cfRule type="expression" dxfId="10" priority="11">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
@@ -2378,7 +2244,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B2" s="32">
         <v>3055</v>
@@ -2393,7 +2259,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B3" s="32">
         <v>3708</v>
@@ -2408,7 +2274,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B4" s="32">
         <v>1339</v>
@@ -2423,7 +2289,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B5" s="32">
         <v>508</v>
@@ -2438,7 +2304,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B6" s="32">
         <v>150</v>
@@ -2458,13 +2324,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2476,7 +2342,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -2505,72 +2371,6 @@
       </c>
       <c r="C3" s="25">
         <v>0.05</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="25">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="25">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="25">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="25">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="25">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="25">
-        <v>0.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sync runbunch data with haag15
</commit_message>
<xml_diff>
--- a/data/runbunch/data.xlsx
+++ b/data/runbunch/data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="600" yWindow="72" windowWidth="22512" windowHeight="9780" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="6" r:id="rId1"/>
@@ -312,7 +312,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -354,6 +354,13 @@
       <i/>
       <sz val="11"/>
       <color theme="6" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -529,9 +536,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -539,12 +544,25 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color theme="5" tint="0.59996337778862885"/>
+      </font>
+    </dxf>
     <dxf>
       <border>
         <top style="thin">
@@ -1331,7 +1349,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,7 +1391,7 @@
       <c r="I1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="35" t="s">
+      <c r="J1" s="33" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1393,7 +1411,7 @@
       <c r="E2" s="3">
         <v>7</v>
       </c>
-      <c r="F2" s="36">
+      <c r="F2" s="34">
         <v>0.01</v>
       </c>
       <c r="G2" s="8">
@@ -1426,7 +1444,7 @@
       <c r="E3" s="3">
         <v>5</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="34">
         <v>0.3</v>
       </c>
       <c r="G3" s="8">
@@ -1459,8 +1477,9 @@
       <c r="E4" s="3">
         <v>8</v>
       </c>
-      <c r="F4" s="36">
-        <v>7.0000000000000007E-2</v>
+      <c r="F4" s="32" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
       </c>
       <c r="G4" s="8">
         <v>2.0000000000000001E-4</v>
@@ -1495,7 +1514,7 @@
         <f>NA()</f>
         <v>#N/A</v>
       </c>
-      <c r="F5" s="34" t="e">
+      <c r="F5" s="32" t="e">
         <f>NA()</f>
         <v>#N/A</v>
       </c>
@@ -1517,13 +1536,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1 A2:B4 J2:XFD4 A5:XFD1048576">
-    <cfRule type="containsErrors" dxfId="12" priority="2">
+    <cfRule type="containsErrors" dxfId="13" priority="3">
       <formula>ISERROR(A1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:I4">
-    <cfRule type="containsErrors" dxfId="11" priority="1">
+  <conditionalFormatting sqref="C2:I3 C4:E4 G4:I4">
+    <cfRule type="containsErrors" dxfId="12" priority="2">
       <formula>ISERROR(C2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F4">
+    <cfRule type="containsErrors" dxfId="0" priority="1">
+      <formula>ISERROR(F4)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -1535,7 +1559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1544,216 +1568,216 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" style="32"/>
-    <col min="3" max="5" width="11.44140625" style="3"/>
-    <col min="6" max="7" width="11.44140625" style="32"/>
-    <col min="8" max="16384" width="11.44140625" style="3"/>
+    <col min="1" max="1" width="23.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" style="40"/>
+    <col min="3" max="5" width="11.44140625" style="41"/>
+    <col min="6" max="7" width="11.44140625" style="40"/>
+    <col min="8" max="16384" width="11.44140625" style="41"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:9" s="37" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="38" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="40">
         <v>20000</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="41">
         <v>100</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="42">
         <v>50</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="43">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="40">
         <v>2000</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="40">
         <v>600000</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="41" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="40">
         <v>0</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="41">
         <v>250</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="42">
         <v>100</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="43">
         <v>0.1</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="40">
         <v>0</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="40">
         <v>50000</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="41" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="40">
         <v>25000</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="41">
         <v>180</v>
       </c>
-      <c r="D4" s="37">
+      <c r="D4" s="42">
         <v>75</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="43">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="40">
         <v>10000</v>
       </c>
-      <c r="G4" s="32">
+      <c r="G4" s="40">
         <v>150000</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="41" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="39" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="40">
         <v>0</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="41">
         <v>250</v>
       </c>
-      <c r="D5" s="37">
+      <c r="D5" s="42">
         <v>75</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="43">
         <v>0.1</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="40">
         <v>0</v>
       </c>
-      <c r="G5" s="32">
+      <c r="G5" s="40">
         <v>50000</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="40">
         <v>30000</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="41">
         <v>60</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="42">
         <v>60</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="43">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="40">
         <v>1000</v>
       </c>
-      <c r="G6" s="32">
+      <c r="G6" s="40">
         <v>500000</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="41" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="39" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="32">
+      <c r="B7" s="40">
         <v>25000</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="41">
         <v>150</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="42">
         <v>50</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="43">
         <v>2.7E-2</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="40">
         <v>500</v>
       </c>
-      <c r="G7" s="32">
+      <c r="G7" s="40">
         <v>350000</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="41" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="32">
+      <c r="B8" s="40">
         <v>0</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="41">
         <v>40</v>
       </c>
-      <c r="D8" s="37">
+      <c r="D8" s="42">
         <v>40</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="43">
         <f>0.023</f>
         <v>2.3E-2</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="40">
         <v>0</v>
       </c>
-      <c r="G8" s="32">
+      <c r="G8" s="40">
         <v>50000</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="41" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1775,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2086,10 +2110,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:XFD5 A8:XFD9 B7:C7 E7:XFD7 B6:XFD6 E10:XFD11 A12:XFD1048576">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>EXACT("In", INDIRECT("Z"&amp;ROW()&amp;"S3",FALSE()))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="12">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2108,23 +2132,23 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D7">
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="9" priority="8">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="9">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="expression" dxfId="6" priority="6">
+    <cfRule type="expression" dxfId="7" priority="6">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:A7">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2143,15 +2167,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:D11">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:A11">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>EXACT(INDIRECT("Z"&amp;(ROW()-1)&amp;"S1",FALSE()),INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE()))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2246,7 +2270,7 @@
       <c r="A2" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="32">
+      <c r="B2" s="31">
         <v>3055</v>
       </c>
       <c r="C2" s="6">
@@ -2255,13 +2279,13 @@
       <c r="D2" s="6">
         <v>0.42</v>
       </c>
-      <c r="E2" s="32"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B3" s="32">
+      <c r="B3" s="31">
         <v>3708</v>
       </c>
       <c r="C3" s="6">
@@ -2270,13 +2294,13 @@
       <c r="D3" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="E3" s="32"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="32">
+      <c r="B4" s="31">
         <v>1339</v>
       </c>
       <c r="C4" s="6">
@@ -2285,13 +2309,13 @@
       <c r="D4" s="6">
         <v>0.1</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="32">
+      <c r="B5" s="31">
         <v>508</v>
       </c>
       <c r="C5" s="6">
@@ -2300,13 +2324,13 @@
       <c r="D5" s="6">
         <v>0.42</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="31">
         <v>150</v>
       </c>
       <c r="C6" s="6">
@@ -2375,7 +2399,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>NOT(EXACT(INDIRECT("Z"&amp;ROW()-1&amp;"S1",FALSE()), INDIRECT("Z"&amp;ROW()&amp;"S1",FALSE())))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>